<commit_message>
RPaM conceptual data model.
</commit_message>
<xml_diff>
--- a/02-Conceptual_Data_Model/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
+++ b/02-Conceptual_Data_Model/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPaM-Ontology_v1.1\02-Conceptual_Data_Model\MS-RPaM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPaM-Ontology\02-Conceptual_Data_Model\MS-RPaM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="392">
   <si>
     <t>This spread-sheet details the content of different MS eMandates and maps it to the RPaM Conceptual Data Model</t>
   </si>
@@ -1201,6 +1201,12 @@
   </si>
   <si>
     <t>Base64</t>
+  </si>
+  <si>
+    <t>eMandateRequest/Criterion</t>
+  </si>
+  <si>
+    <t>Criteria, in the eMandateRequest are used to specify Service Provider adhoc information Requirements (IR). This need (OAFriendlyName) is seen as an SP-IR.</t>
   </si>
 </sst>
 </file>
@@ -1697,6 +1703,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1721,15 +1731,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="2" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
+    <cellStyle name="Notas" xfId="2" builtinId="10"/>
+    <cellStyle name="Texto de advertencia" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1745,7 +1751,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2013,7 +2019,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -2038,7 +2044,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -2053,23 +2059,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="78" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="41"/>
       <c r="I2" s="42"/>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
@@ -2926,11 +2932,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="4.140625" customWidth="1"/>
@@ -2949,22 +2955,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="78" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -3011,7 +3017,7 @@
       <c r="O3" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="83" t="s">
+      <c r="P3" s="75" t="s">
         <v>386</v>
       </c>
     </row>
@@ -3037,7 +3043,7 @@
       <c r="J4" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="81" t="s">
+      <c r="K4" s="73" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="9" t="s">
@@ -3068,13 +3074,13 @@
       <c r="H5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="76" t="s">
         <v>388</v>
       </c>
       <c r="J5" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="74" t="s">
         <v>389</v>
       </c>
       <c r="L5" s="13"/>
@@ -3100,11 +3106,17 @@
       <c r="H6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="82"/>
+      <c r="I6" s="76" t="s">
+        <v>390</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="K6" s="74"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="N6" s="13"/>
       <c r="O6" s="16"/>
     </row>
@@ -3126,7 +3138,7 @@
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="82"/>
+      <c r="K7" s="74"/>
       <c r="L7" s="13"/>
       <c r="M7" s="14"/>
       <c r="N7" s="13"/>
@@ -3152,7 +3164,7 @@
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="82"/>
+      <c r="K8" s="74"/>
       <c r="L8" s="13"/>
       <c r="M8" s="14"/>
       <c r="N8" s="13"/>
@@ -3172,7 +3184,7 @@
       <c r="H9" s="25"/>
       <c r="I9" s="12"/>
       <c r="J9" s="13"/>
-      <c r="K9" s="82"/>
+      <c r="K9" s="74"/>
       <c r="L9" s="13"/>
       <c r="M9" s="14"/>
       <c r="N9" s="13"/>
@@ -3192,7 +3204,7 @@
       <c r="H10" s="25"/>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="82"/>
+      <c r="K10" s="74"/>
       <c r="L10" s="13"/>
       <c r="M10" s="14"/>
       <c r="N10" s="13"/>
@@ -3212,7 +3224,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="12"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="82"/>
+      <c r="K11" s="74"/>
       <c r="L11" s="13"/>
       <c r="M11" s="14"/>
       <c r="N11" s="13"/>
@@ -3232,7 +3244,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="82"/>
+      <c r="K12" s="74"/>
       <c r="L12" s="13"/>
       <c r="M12" s="14"/>
       <c r="N12" s="13"/>
@@ -3260,7 +3272,7 @@
       <c r="J13" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="82" t="s">
+      <c r="K13" s="74" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="13" t="s">
@@ -3292,7 +3304,7 @@
         <v>58</v>
       </c>
       <c r="J14" s="13"/>
-      <c r="K14" s="82" t="s">
+      <c r="K14" s="74" t="s">
         <v>28</v>
       </c>
       <c r="L14" s="13" t="s">
@@ -3328,7 +3340,7 @@
         <v>63</v>
       </c>
       <c r="J15" s="13"/>
-      <c r="K15" s="82" t="s">
+      <c r="K15" s="74" t="s">
         <v>28</v>
       </c>
       <c r="L15" s="13" t="s">
@@ -3362,7 +3374,7 @@
       <c r="J16" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="82" t="s">
+      <c r="K16" s="74" t="s">
         <v>21</v>
       </c>
       <c r="L16" s="13" t="s">
@@ -3394,7 +3406,7 @@
       <c r="J17" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="74" t="s">
         <v>21</v>
       </c>
       <c r="L17" s="13" t="s">
@@ -4148,7 +4160,7 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="5.140625" customWidth="1"/>
@@ -4166,22 +4178,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="78" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -5078,7 +5090,7 @@
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" customWidth="1"/>
@@ -5097,22 +5109,22 @@
   <sheetData>
     <row r="1" spans="2:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="78" t="s">
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
       <c r="N3" s="4"/>
       <c r="O3" s="7"/>
     </row>
@@ -6620,7 +6632,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
@@ -6637,22 +6649,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="78" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -6946,7 +6958,7 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.140625" customWidth="1"/>
@@ -6965,22 +6977,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="79" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>

</xml_diff>

<commit_message>
MS-RPaM-Mapping, new elements and business rules.
</commit_message>
<xml_diff>
--- a/02-Conceptual_Data_Model/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
+++ b/02-Conceptual_Data_Model/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="467">
   <si>
     <t>This spread-sheet details the content of different MS eMandates and maps it to the RPaM Conceptual Data Model</t>
   </si>
@@ -1209,33 +1209,18 @@
     <t>Criteria, in the eMandateRequest are used to specify Service Provider adhoc information Requirements (IR). This need (OAFriendlyName) is seen as an SP-IR.</t>
   </si>
   <si>
-    <t>TBD with AT</t>
-  </si>
-  <si>
     <t>eMandateRequest/Mandate/id</t>
   </si>
   <si>
     <t>The identifier(s) of the mandate</t>
   </si>
   <si>
-    <t>What for? TBD with AT</t>
-  </si>
-  <si>
-    <t>What does "target" refer to?</t>
-  </si>
-  <si>
-    <t>What would we need this in the exchanged document.</t>
-  </si>
-  <si>
     <t>The idea of accessing this datum online is interesting, but if the objective is to check it at real time, in our Use Case this would not be necessary as the mandate is retrieved directly from the eMandate Registry, without any intervention by the user. Thus the status is a "real-time" one.</t>
   </si>
   <si>
     <t>TBD AT</t>
   </si>
   <si>
-    <t>eMandateRequest/Mandate/Empowerment/Description</t>
-  </si>
-  <si>
     <t>xsd:String</t>
   </si>
   <si>
@@ -1245,26 +1230,218 @@
     <t>ccts:Text</t>
   </si>
   <si>
-    <t>eMandateRequest/Mandate/Empowerment/statusType</t>
-  </si>
-  <si>
-    <t>eMandateRequest/Mandate/Empowerment/Mandatee</t>
-  </si>
-  <si>
     <t>rpam:Mandatee</t>
   </si>
   <si>
     <t xml:space="preserve">The ontology is able to infer the type of person based on its type. In UBL we need to have to different ASBIEs, as in AT (see examples under folder 03-Syntax_Bindings/OWL-DL-TTL/examples and 03-Syntax_Bindings/UBL-NDR-BASED/examples </t>
   </si>
   <si>
-    <t>What is the difference between physical and corporate? The definitions do not give a hint.</t>
+    <t>The organization that mandated this person to represent it.</t>
+  </si>
+  <si>
+    <t>The empowered person.</t>
+  </si>
+  <si>
+    <t>The mandate of a mandator that is delegating its power onto another mandatee.</t>
+  </si>
+  <si>
+    <t>A proxy, as defined in Deliverable 1?</t>
+  </si>
+  <si>
+    <t>eR*/Mandate/Empowerment/Description</t>
+  </si>
+  <si>
+    <t>eMandateRequest</t>
+  </si>
+  <si>
+    <t>eRR stands for eMandateRequest and eMandateResponse</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/ID</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/statusType</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/Mandatee</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/Intermediary</t>
+  </si>
+  <si>
+    <t>eRR/id</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/id</t>
+  </si>
+  <si>
+    <t>eRR/IssueDateTime</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Description</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/hasPower/Power/FinancialTheresholdConstraint</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/lifeSpan</t>
+  </si>
+  <si>
+    <t>ubl:Period</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/Mandatee/Organization</t>
+  </si>
+  <si>
+    <t>org:Organization</t>
+  </si>
+  <si>
+    <t>Could belong to more than one organization</t>
+  </si>
+  <si>
+    <t>The attributes schemeID, schemeAgencyID should be compulsory for the Request and Response documents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The attributes of the document id should be sufficient to identify who issued the document. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The attributes of the mandate id should be sufficient to identify the registry where the mandate was created. </t>
+  </si>
+  <si>
+    <t>The attributes schemeID, schemeAgencyID should be compulsory for the Mandate</t>
+  </si>
+  <si>
+    <t>The identifier(s) of the eBusiness Document (transaction)</t>
+  </si>
+  <si>
+    <t>The identifier(s) of the mandate (the empowerment container)</t>
+  </si>
+  <si>
+    <t>The date and time of the eBusiness Document</t>
+  </si>
+  <si>
+    <t>The lifecycle of the mandate in the eMandate Registry where it is kept.</t>
+  </si>
+  <si>
+    <t>The creation date and the struck-off date.</t>
+  </si>
+  <si>
+    <t>Both date and time must be compulsory in this case, as this is a systemic timestamp.</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/MandatorConstraint</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/Constraint(s)</t>
+  </si>
+  <si>
+    <t>The constraints applied to the use of the power by mandator and mandatees.</t>
+  </si>
+  <si>
+    <t>See triples rpam:Empowerment rpam:mandator ccev:Constraint and rpam:Empowerment rpam:mandatee ccev:Constraint</t>
+  </si>
+  <si>
+    <t>DEFINITION NEEDED</t>
+  </si>
+  <si>
+    <t>ccev:CriterionProperty</t>
+  </si>
+  <si>
+    <t>Cover by RPaM as a CriterionProperty of type xsd:boolean (ccts:Indicator in UBL)</t>
+  </si>
+  <si>
+    <t>Constraints applied to the Mandate that affect all the empowerments therein  contained. These constraints shoud be commonly shared through a register of SP-Information Requirements and Constraints (e.g. eCertis).</t>
+  </si>
+  <si>
+    <t>We want avoid the perverse effects of the "other" approach. This hampers terribly the interoperability. Our proposal is to register and share any constraint that may be reused. If the constraint is of national or administration scope, then the IR and Constraint Register should cater for the definition of sub-criteria based on the common global constraints, as in eCertis.</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Constraint</t>
+  </si>
+  <si>
+    <t>For data protection and privacy reasons, as the mandate can contain multiple empowerments to other persons, the eMandate Registry must make sure that the eMandate Response contains only information about the empowerment of the person concerned in the Request. This rule should apply to mandatees that are both Natural and Legal Persons.</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/Mandatee/RelatedMandate</t>
+  </si>
+  <si>
+    <t>eRR/Mandate/Empowerment/Mandator/RelatedMandate</t>
+  </si>
+  <si>
+    <t>@everis:For all rows in this spread-sheet we need to re-check whether the requirement applies to both documents or just to one of them</t>
+  </si>
+  <si>
+    <t>@AT: We need more insight on the meaning of "substituable" from AT.</t>
+  </si>
+  <si>
+    <t>@AT: please, what is the difference between a Mandate and a SimpleMandate?</t>
+  </si>
+  <si>
+    <t>@AT: We do not understand how this is used. AT, can you explain,  please? And provide examples?</t>
+  </si>
+  <si>
+    <t>@AT: Do you refer to the constraints of the mandator's and mandatee's use of the power in an empowerment? Otherwise can you explain and PROVIDE EXAMPLES, please?</t>
+  </si>
+  <si>
+    <t>@everis: 1. Add to the ontology. 2. Update the configuration  matrix.</t>
+  </si>
+  <si>
+    <t>@AT: Can you elaborate plelase? @everis: 1. We need to understand well this need, but we can already add it to the Ontology. I have the gut-feeling that we'll need it. I see it in the empowerment. BTW I thing we have the definition in the glossary.</t>
+  </si>
+  <si>
+    <t>@everis: 1. Move the delegationLevel to Empowerment
+2. Add a new constraint to the GenericConstraint: "The power cannot be delegated".
+3. Simplify the model like this: rpam:Empowerment rpam:constraint ccev:CriterionProperty. 4. Update the Configuration Matrix</t>
+  </si>
+  <si>
+    <t>@AT: 1. We think that the need AT has is in reality to be able to access the organisation to which a person works for. Are we mistaken?
+2. Update the configuration matrix.</t>
+  </si>
+  <si>
+    <t>@everis: 1. Add this element to the Ontology. 2. Update the configuration matrix.</t>
+  </si>
+  <si>
+    <t>@AT: TBD</t>
+  </si>
+  <si>
+    <t>@AT: What for?</t>
+  </si>
+  <si>
+    <t>@AT: What does "target" refer to?</t>
+  </si>
+  <si>
+    <t>@AT: Why would we need this in the exchanged document.</t>
+  </si>
+  <si>
+    <t>eMandateResponse/Mandate/ValidityPeriodConstraint</t>
+  </si>
+  <si>
+    <t>The period of time the power can be used by the mandatee.</t>
+  </si>
+  <si>
+    <t>If not present then it does not expire (until the empowerment is revoked or the mandate struck-off).</t>
+  </si>
+  <si>
+    <t>@everis: 1. Add to the matrix configuration the need to document that "If a mandate is struck-off in the eMandate Registry, all the empowerments therein contained must change their statuses accordingly (we may need to come up with a new status named :CANCELLED_MANDATE_STRUCK_OFF</t>
+  </si>
+  <si>
+    <t>@everis: we may need a code list for the types of Mandates (simple, collective, ….)</t>
+  </si>
+  <si>
+    <t>We think this is solved in our model, and that it can be controlled via the Mandate Type</t>
+  </si>
+  <si>
+    <t>We think this is not necessary in a trusted environment. The pilot should bring on board the e-Delivery four corners approach.</t>
+  </si>
+  <si>
+    <t>@AT: can we agree on this?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1331,8 +1508,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1639,7 +1824,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1676,9 +1861,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1694,7 +1876,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1742,9 +1923,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -1766,14 +1944,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1798,8 +1974,77 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2128,23 +2373,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="72" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="78" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
@@ -2162,7 +2407,7 @@
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="51" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -2171,19 +2416,19 @@
       <c r="I3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="35" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2206,11 +2451,11 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="31"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
@@ -2233,13 +2478,13 @@
         <v>165</v>
       </c>
       <c r="I5" s="15"/>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -2262,13 +2507,13 @@
       <c r="I6" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="J6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="36"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
@@ -2289,13 +2534,13 @@
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="15"/>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
@@ -2318,11 +2563,11 @@
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="15"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
@@ -2341,11 +2586,11 @@
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="15"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
@@ -2370,15 +2615,15 @@
       <c r="I10" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="35"/>
-    </row>
-    <row r="11" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="33"/>
+    </row>
+    <row r="11" spans="2:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
@@ -2394,12 +2639,12 @@
         <v>37</v>
       </c>
       <c r="H11" s="21"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
@@ -2424,15 +2669,15 @@
       <c r="I12" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="35"/>
-    </row>
-    <row r="13" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="33"/>
+    </row>
+    <row r="13" spans="2:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>12</v>
       </c>
@@ -2448,14 +2693,14 @@
         <v>46</v>
       </c>
       <c r="H13" s="21"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-    </row>
-    <row r="14" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="37"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+    </row>
+    <row r="14" spans="2:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>12</v>
       </c>
@@ -2471,12 +2716,12 @@
         <v>46</v>
       </c>
       <c r="H14" s="21"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
@@ -2495,13 +2740,13 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
@@ -2522,13 +2767,13 @@
       <c r="I16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="35" t="s">
+      <c r="J16" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="33"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
@@ -2547,11 +2792,11 @@
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="16"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
@@ -2578,13 +2823,13 @@
       <c r="I18" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="35" t="s">
+      <c r="J18" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
@@ -2609,49 +2854,49 @@
       <c r="I19" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="35" t="s">
+      <c r="J19" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="31"/>
     </row>
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="62" t="s">
+      <c r="G20" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="61" t="s">
+      <c r="H20" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="I20" s="63" t="s">
+      <c r="I20" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="J20" s="64" t="s">
+      <c r="J20" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="K20" s="65"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="65"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="62"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C21" s="21" t="s">
@@ -2665,14 +2910,14 @@
       <c r="G21" s="14"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -2692,14 +2937,14 @@
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="21" t="s">
@@ -2717,14 +2962,14 @@
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -2742,14 +2987,14 @@
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -2765,14 +3010,14 @@
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -2790,14 +3035,14 @@
       </c>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C27" s="21" t="s">
@@ -2813,14 +3058,14 @@
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C28" s="21" t="s">
@@ -2836,14 +3081,14 @@
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -2859,14 +3104,14 @@
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C30" s="13" t="s">
@@ -2880,14 +3125,14 @@
       <c r="G30" s="14"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="59"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -2903,14 +3148,14 @@
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59"/>
-      <c r="N31" s="59"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -2930,14 +3175,14 @@
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="59"/>
-      <c r="M32" s="59"/>
-      <c r="N32" s="59"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="36" t="s">
         <v>234</v>
       </c>
       <c r="C33" s="13" t="s">
@@ -2954,38 +3199,38 @@
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
-      <c r="J33" s="71"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="59"/>
-      <c r="M33" s="59"/>
-      <c r="N33" s="59"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
     </row>
     <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="64" t="s">
         <v>234</v>
       </c>
-      <c r="C34" s="68" t="s">
+      <c r="C34" s="65" t="s">
         <v>337</v>
       </c>
-      <c r="D34" s="61" t="s">
+      <c r="D34" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="E34" s="61" t="s">
+      <c r="E34" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="61" t="s">
+      <c r="F34" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="62" t="s">
+      <c r="G34" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="61"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2999,1270 +3244,1544 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P46"/>
+  <dimension ref="B1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="89" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="89" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" style="89" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="89" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="89" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="90" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.28515625" style="89" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="89" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="89" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" style="89" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="90" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="89"/>
+    <col min="15" max="15" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="89" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="89"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C1" s="97" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="83" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="121"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H4" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J4" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K4" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L4" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="72" t="s">
+      <c r="M4" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N4" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="23" t="s">
+      <c r="O4" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="75" t="s">
+      <c r="P4" s="84" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="27" t="s">
+    <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="91"/>
+      <c r="C5" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D5" s="92" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E5" s="92" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="26">
+      <c r="F5" s="92"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="94">
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I5" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J5" s="98" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K5" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L5" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M5" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="32"/>
-      <c r="P4" t="s">
+      <c r="N5" s="98"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="89" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="21" t="s">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="96"/>
+      <c r="C6" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D6" s="97" t="s">
         <v>148</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E6" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="25" t="s">
+      <c r="F6" s="97"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="76" t="s">
+      <c r="I6" s="85" t="s">
         <v>388</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J6" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="K6" s="86" t="s">
         <v>389</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L6" s="98" t="s">
+        <v>397</v>
+      </c>
+      <c r="M6" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" s="98"/>
+      <c r="O6" s="114"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="96"/>
+      <c r="C7" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D7" s="97" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="97" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="97"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="85" t="s">
+        <v>390</v>
+      </c>
+      <c r="J7" s="97" t="s">
+        <v>391</v>
+      </c>
+      <c r="K7" s="86"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="98"/>
+      <c r="O7" s="114"/>
+      <c r="P7" s="123" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="96"/>
+      <c r="C8" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D8" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="98" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="99">
+        <v>1</v>
+      </c>
+      <c r="I8" s="88" t="s">
+        <v>395</v>
+      </c>
+      <c r="J8" s="98"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="100"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="114"/>
+      <c r="P8" s="123" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="96"/>
+      <c r="C9" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D9" s="97" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="97" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="98" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="98"/>
+      <c r="H9" s="99">
+        <v>1</v>
+      </c>
+      <c r="I9" s="88" t="s">
+        <v>395</v>
+      </c>
+      <c r="J9" s="98"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="100"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="123" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="96"/>
+      <c r="C10" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D10" s="97" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="89" t="s">
+        <v>392</v>
+      </c>
+      <c r="J10" s="97" t="s">
+        <v>393</v>
+      </c>
+      <c r="K10" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="93" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="95" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="98"/>
+      <c r="O10" s="114"/>
+      <c r="P10" s="87"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="96"/>
+      <c r="C11" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D11" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="88" t="s">
+        <v>395</v>
+      </c>
+      <c r="J11" s="98"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="114"/>
+      <c r="P11" s="123" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="96"/>
+      <c r="C12" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="88" t="s">
+        <v>395</v>
+      </c>
+      <c r="J12" s="98"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="114"/>
+      <c r="P12" s="123" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="96"/>
+      <c r="C13" s="97" t="s">
+        <v>406</v>
+      </c>
+      <c r="D13" s="97" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="88" t="s">
+        <v>395</v>
+      </c>
+      <c r="J13" s="98"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="114"/>
+      <c r="P13" s="123" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="97" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="98"/>
+      <c r="H14" s="99">
+        <v>1</v>
+      </c>
+      <c r="I14" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="J14" s="98" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="98"/>
+      <c r="O14" s="114"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="96"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="97" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="98"/>
+      <c r="H15" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="85" t="s">
+        <v>405</v>
+      </c>
+      <c r="J15" s="98"/>
+      <c r="K15" s="86" t="s">
+        <v>398</v>
+      </c>
+      <c r="L15" s="86" t="s">
+        <v>396</v>
+      </c>
+      <c r="M15" s="102">
+        <v>1</v>
+      </c>
+      <c r="N15" s="98" t="s">
+        <v>62</v>
+      </c>
+      <c r="O15" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="P15" s="123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="97" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="98"/>
+      <c r="H16" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="J16" s="98"/>
+      <c r="K16" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="102">
+        <v>1</v>
+      </c>
+      <c r="N16" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="O16" s="115" t="s">
+        <v>394</v>
+      </c>
+      <c r="P16" s="113" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="98" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="99">
+        <v>1</v>
+      </c>
+      <c r="I17" s="96" t="s">
+        <v>410</v>
+      </c>
+      <c r="J17" s="98"/>
+      <c r="K17" s="86" t="s">
+        <v>399</v>
+      </c>
+      <c r="L17" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="115" t="s">
+        <v>400</v>
+      </c>
+      <c r="P17" s="113" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="165" x14ac:dyDescent="0.25">
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="98" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="99">
+        <v>1</v>
+      </c>
+      <c r="I18" s="85" t="s">
+        <v>419</v>
+      </c>
+      <c r="J18" s="98" t="s">
+        <v>401</v>
+      </c>
+      <c r="K18" s="86" t="s">
+        <v>420</v>
+      </c>
+      <c r="L18" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" s="98"/>
+      <c r="O18" s="115" t="s">
+        <v>421</v>
+      </c>
+      <c r="P18" s="124" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="98" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="98" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="99">
+        <v>1</v>
+      </c>
+      <c r="I19" s="96" t="s">
+        <v>410</v>
+      </c>
+      <c r="J19" s="98" t="s">
         <v>402</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="K19" s="98" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" s="98"/>
+      <c r="M19" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="98"/>
+      <c r="O19" s="114"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="97" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="97" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="97"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="99">
+        <v>1</v>
+      </c>
+      <c r="I20" s="85" t="s">
+        <v>444</v>
+      </c>
+      <c r="J20" s="97" t="s">
+        <v>403</v>
+      </c>
+      <c r="K20" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" s="98"/>
+      <c r="M20" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" s="98"/>
+      <c r="O20" s="116"/>
+      <c r="P20" s="123" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="96"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="25" t="s">
+      <c r="I21" s="85" t="s">
+        <v>411</v>
+      </c>
+      <c r="J21" s="97" t="s">
+        <v>404</v>
+      </c>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21" s="98"/>
+      <c r="O21" s="114"/>
+      <c r="P21" s="123" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="96"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="98" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="98" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="98"/>
+      <c r="H22" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="96" t="s">
+        <v>412</v>
+      </c>
+      <c r="J22" s="97" t="s">
+        <v>426</v>
+      </c>
+      <c r="K22" s="98"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="100">
+        <v>1</v>
+      </c>
+      <c r="N22" s="85" t="s">
+        <v>422</v>
+      </c>
+      <c r="O22" s="115" t="s">
+        <v>423</v>
+      </c>
+      <c r="P22" s="112" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="96"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="98" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="98" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="98"/>
+      <c r="H23" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="96" t="s">
+        <v>413</v>
+      </c>
+      <c r="J23" s="97" t="s">
+        <v>427</v>
+      </c>
+      <c r="K23" s="98"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="100">
+        <v>1</v>
+      </c>
+      <c r="N23" s="85" t="s">
+        <v>425</v>
+      </c>
+      <c r="O23" s="115" t="s">
+        <v>424</v>
+      </c>
+      <c r="P23" s="112" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="96"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="98" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="98" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="98" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="96" t="s">
+        <v>414</v>
+      </c>
+      <c r="J24" s="97" t="s">
+        <v>428</v>
+      </c>
+      <c r="K24" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="98" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="100">
+        <v>1</v>
+      </c>
+      <c r="N24" s="85" t="s">
+        <v>431</v>
+      </c>
+      <c r="O24" s="114" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="96"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="98" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="98" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="96" t="s">
+        <v>417</v>
+      </c>
+      <c r="J25" s="97" t="s">
+        <v>429</v>
+      </c>
+      <c r="K25" s="98" t="s">
+        <v>418</v>
+      </c>
+      <c r="L25" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" s="100">
+        <v>1</v>
+      </c>
+      <c r="N25" s="85" t="s">
+        <v>431</v>
+      </c>
+      <c r="O25" s="115" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="96"/>
+      <c r="C26" s="97"/>
+      <c r="D26" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="76" t="s">
-        <v>390</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="K6" s="74"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="5" t="s">
+      <c r="I26" s="96" t="s">
+        <v>433</v>
+      </c>
+      <c r="J26" s="97" t="s">
+        <v>434</v>
+      </c>
+      <c r="K26" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L26" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="M26" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="77" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="25">
+      <c r="N26" s="98"/>
+      <c r="O26" s="114" t="s">
+        <v>435</v>
+      </c>
+      <c r="P26" s="112" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="96"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="98" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="98" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="96" t="s">
+        <v>432</v>
+      </c>
+      <c r="J27" s="85" t="s">
+        <v>436</v>
+      </c>
+      <c r="K27" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L27" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="M27" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" s="98"/>
+      <c r="O27" s="114" t="s">
+        <v>438</v>
+      </c>
+      <c r="P27" s="112" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="96"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="98" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="98" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="J28" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="K28" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L28" s="98"/>
+      <c r="M28" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N28" s="98"/>
+      <c r="O28" s="114" t="s">
+        <v>440</v>
+      </c>
+      <c r="P28" s="97" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="96"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="98" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="98" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="98" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="98"/>
+      <c r="H29" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="96" t="s">
+        <v>415</v>
+      </c>
+      <c r="J29" s="98"/>
+      <c r="K29" s="98" t="s">
+        <v>102</v>
+      </c>
+      <c r="L29" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="M29" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" s="98"/>
+      <c r="O29" s="114"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="96"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="98" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="96" t="s">
+        <v>415</v>
+      </c>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98" t="s">
+        <v>102</v>
+      </c>
+      <c r="L30" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" s="98"/>
+      <c r="O30" s="114"/>
+      <c r="P30" s="112" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="96"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="98" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="98" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="96" t="s">
+        <v>444</v>
+      </c>
+      <c r="J31" s="97" t="s">
+        <v>403</v>
+      </c>
+      <c r="K31" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="L31" s="98"/>
+      <c r="M31" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="N31" s="98"/>
+      <c r="O31" s="116"/>
+      <c r="P31" s="123" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="96"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="98" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="98" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="85" t="s">
+        <v>443</v>
+      </c>
+      <c r="J32" s="97" t="s">
+        <v>403</v>
+      </c>
+      <c r="K32" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="98"/>
+      <c r="M32" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" s="85" t="s">
+        <v>442</v>
+      </c>
+      <c r="O32" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="P32" s="123" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="96"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="98" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="98" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="98"/>
+      <c r="G33" s="98"/>
+      <c r="H33" s="99" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="J33" s="98" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="98" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="N33" s="98"/>
+      <c r="O33" s="114"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="96"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="98" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="98" t="s">
+        <v>138</v>
+      </c>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="J34" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="K34" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L34" s="98"/>
+      <c r="M34" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N34" s="98"/>
+      <c r="O34" s="114" t="s">
+        <v>440</v>
+      </c>
+      <c r="P34" s="97" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="96"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="98" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="98" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="96" t="s">
+        <v>459</v>
+      </c>
+      <c r="J35" s="97" t="s">
+        <v>460</v>
+      </c>
+      <c r="K35" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="L35" s="97" t="s">
+        <v>418</v>
+      </c>
+      <c r="M35" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="N35" s="98"/>
+      <c r="O35" s="114" t="s">
+        <v>461</v>
+      </c>
+      <c r="P35" s="112" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="96"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="98" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="J36" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="K36" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L36" s="98"/>
+      <c r="M36" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N36" s="98"/>
+      <c r="O36" s="114" t="s">
+        <v>464</v>
+      </c>
+      <c r="P36" s="112" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="96"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="98" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="98"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="98"/>
+      <c r="H37" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="J37" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="K37" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L37" s="98"/>
+      <c r="M37" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N37" s="98"/>
+      <c r="O37" s="114" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="96"/>
+      <c r="C38" s="97"/>
+      <c r="D38" s="98" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="J38" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="K38" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L38" s="98"/>
+      <c r="M38" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N38" s="98"/>
+      <c r="O38" s="114" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="96"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="98" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39" s="98" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="98"/>
+      <c r="G39" s="98"/>
+      <c r="H39" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="104" t="s">
+        <v>416</v>
+      </c>
+      <c r="J39" s="97"/>
+      <c r="K39" s="97" t="s">
+        <v>175</v>
+      </c>
+      <c r="L39" s="97"/>
+      <c r="M39" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="N39" s="97"/>
+      <c r="O39" s="117"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="96"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="98" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="98" t="s">
+        <v>142</v>
+      </c>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="I40" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="J40" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="K40" s="97" t="s">
+        <v>437</v>
+      </c>
+      <c r="L40" s="98"/>
+      <c r="M40" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="N40" s="98"/>
+      <c r="O40" s="114"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="105"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="107" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="107" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="107"/>
+      <c r="G41" s="107"/>
+      <c r="H41" s="108">
         <v>1</v>
       </c>
-      <c r="I7" s="86" t="s">
-        <v>399</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="77" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="25">
-        <v>1</v>
-      </c>
-      <c r="I8" s="86" t="s">
-        <v>399</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="77" t="s">
+      <c r="I41" s="125" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="25"/>
-      <c r="I9" t="s">
-        <v>393</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>394</v>
-      </c>
-      <c r="K9" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="10" t="s">
+      <c r="J41" s="107"/>
+      <c r="K41" s="107"/>
+      <c r="L41" s="107"/>
+      <c r="M41" s="109"/>
+      <c r="N41" s="107"/>
+      <c r="O41" s="118" t="s">
+        <v>465</v>
+      </c>
+      <c r="P41" s="112" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="91"/>
+      <c r="C42" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="D42" s="92" t="s">
+        <v>305</v>
+      </c>
+      <c r="E42" s="92" t="s">
+        <v>313</v>
+      </c>
+      <c r="F42" s="93" t="s">
+        <v>43</v>
+      </c>
+      <c r="G42" s="93"/>
+      <c r="H42" s="94"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="93"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="95"/>
+      <c r="N42" s="93"/>
+      <c r="O42" s="111"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="96"/>
+      <c r="C43" s="98" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" s="97" t="s">
+        <v>306</v>
+      </c>
+      <c r="E43" s="97" t="s">
+        <v>314</v>
+      </c>
+      <c r="F43" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="G43" s="98"/>
+      <c r="H43" s="99"/>
+      <c r="I43" s="96"/>
+      <c r="J43" s="98"/>
+      <c r="K43" s="98"/>
+      <c r="L43" s="98"/>
+      <c r="M43" s="100"/>
+      <c r="N43" s="98"/>
+      <c r="O43" s="101"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="96"/>
+      <c r="C44" s="98" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44" s="97" t="s">
+        <v>308</v>
+      </c>
+      <c r="E44" s="97" t="s">
+        <v>319</v>
+      </c>
+      <c r="F44" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" s="98"/>
+      <c r="H44" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="77"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="86" t="s">
-        <v>399</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="77" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="86" t="s">
-        <v>399</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="77" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="86" t="s">
-        <v>399</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="77" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="25">
-        <v>1</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="N13" s="13"/>
-      <c r="O13" s="15"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="76" t="s">
-        <v>400</v>
-      </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="74" t="s">
-        <v>403</v>
-      </c>
-      <c r="L14" s="74" t="s">
-        <v>401</v>
-      </c>
-      <c r="M14" s="5">
-        <v>1</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O14" s="87" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>404</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M15" s="5">
-        <v>1</v>
-      </c>
-      <c r="N15" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="O15" s="87" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="25">
-        <v>1</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>405</v>
-      </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="74" t="s">
-        <v>406</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O16" s="87" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="25">
-        <v>1</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>405</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="K17" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="N17" s="13"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="77" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="25">
-        <v>1</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13" t="s">
+      <c r="I44" s="97" t="s">
+        <v>327</v>
+      </c>
+      <c r="J44" s="98" t="s">
+        <v>38</v>
+      </c>
+      <c r="K44" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="L18" s="13"/>
-      <c r="M18" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="16"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="25">
-        <v>1</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="16"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="15"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="25">
-        <v>1</v>
-      </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="15"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="H22" s="25">
-        <v>1</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M22" s="14">
-        <v>1</v>
-      </c>
-      <c r="N22" s="13"/>
-      <c r="O22" s="15"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="H23" s="25">
-        <v>1</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M23" s="14">
-        <v>1</v>
-      </c>
-      <c r="N23" s="13"/>
-      <c r="O23" s="15"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="15"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="15"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="15"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="13"/>
-      <c r="H27" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N27" s="13"/>
-      <c r="O27" s="15"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N28" s="13"/>
-      <c r="O28" s="15"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="15"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="25" t="s">
+      <c r="L44" s="98"/>
+      <c r="M44" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="N30" s="13"/>
-      <c r="O30" s="15"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="15"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="15"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="15"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="15"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="15"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="12"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="L36" s="21"/>
-      <c r="M36" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="N36" s="21"/>
-      <c r="O36" s="39"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="12"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="15"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="17"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="30">
-        <v>1</v>
-      </c>
-      <c r="I38" s="17"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="31"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
-      <c r="C39" s="9" t="s">
+      <c r="N44" s="98"/>
+      <c r="O44" s="101"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="96"/>
+      <c r="C45" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="D39" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="E39" s="27" t="s">
-        <v>313</v>
-      </c>
-      <c r="F39" s="9" t="s">
+      <c r="D45" s="97" t="s">
+        <v>307</v>
+      </c>
+      <c r="E45" s="98" t="s">
+        <v>318</v>
+      </c>
+      <c r="F45" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="11"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="12"/>
-      <c r="C40" s="13" t="s">
+      <c r="G45" s="98"/>
+      <c r="H45" s="99" t="s">
+        <v>37</v>
+      </c>
+      <c r="I45" s="96"/>
+      <c r="J45" s="98"/>
+      <c r="K45" s="98"/>
+      <c r="L45" s="98"/>
+      <c r="M45" s="100"/>
+      <c r="N45" s="98"/>
+      <c r="O45" s="101"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="96"/>
+      <c r="C46" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="D40" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>314</v>
-      </c>
-      <c r="F40" s="21" t="s">
+      <c r="D46" s="97" t="s">
+        <v>309</v>
+      </c>
+      <c r="E46" s="98" t="s">
+        <v>317</v>
+      </c>
+      <c r="F46" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="G40" s="13"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="12"/>
-      <c r="C41" s="13" t="s">
+      <c r="G46" s="98"/>
+      <c r="H46" s="99"/>
+      <c r="I46" s="96"/>
+      <c r="J46" s="98"/>
+      <c r="K46" s="98"/>
+      <c r="L46" s="98"/>
+      <c r="M46" s="100"/>
+      <c r="N46" s="98"/>
+      <c r="O46" s="101"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="96"/>
+      <c r="C47" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="D41" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>319</v>
-      </c>
-      <c r="F41" s="21" t="s">
+      <c r="D47" s="97" t="s">
+        <v>310</v>
+      </c>
+      <c r="E47" s="98"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="98"/>
+      <c r="H47" s="99"/>
+      <c r="I47" s="96"/>
+      <c r="J47" s="98"/>
+      <c r="K47" s="98"/>
+      <c r="L47" s="98"/>
+      <c r="M47" s="100"/>
+      <c r="N47" s="98"/>
+      <c r="O47" s="101"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="96"/>
+      <c r="C48" s="98" t="s">
+        <v>234</v>
+      </c>
+      <c r="D48" s="97" t="s">
+        <v>311</v>
+      </c>
+      <c r="E48" s="98" t="s">
+        <v>315</v>
+      </c>
+      <c r="F48" s="98"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="99"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="98"/>
+      <c r="M48" s="100"/>
+      <c r="N48" s="98"/>
+      <c r="O48" s="101"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="105"/>
+      <c r="C49" s="107" t="s">
+        <v>234</v>
+      </c>
+      <c r="D49" s="106" t="s">
+        <v>312</v>
+      </c>
+      <c r="E49" s="107" t="s">
+        <v>316</v>
+      </c>
+      <c r="F49" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="13"/>
-      <c r="H41" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="I41" s="21" t="s">
-        <v>327</v>
-      </c>
-      <c r="J41" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L41" s="13"/>
-      <c r="M41" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N41" s="13"/>
-      <c r="O41" s="15"/>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="12"/>
-      <c r="C42" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="F42" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="15"/>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="12"/>
-      <c r="C43" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="F43" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="15"/>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="12"/>
-      <c r="C44" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="15"/>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="12"/>
-      <c r="C45" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="15"/>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="17"/>
-      <c r="C46" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G46" s="18"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="31"/>
+      <c r="G49" s="107"/>
+      <c r="H49" s="108"/>
+      <c r="I49" s="105"/>
+      <c r="J49" s="107"/>
+      <c r="K49" s="107"/>
+      <c r="L49" s="107"/>
+      <c r="M49" s="109"/>
+      <c r="N49" s="107"/>
+      <c r="O49" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="I3:M3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" display="eR@ stands for eMandateRequest and eMandateResponse"/>
+    <hyperlink ref="P32" r:id="rId2" display="0@AT, please, what is the difference between a Mandate and a SimpleMandate?"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4292,22 +4811,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="83" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -4360,13 +4879,13 @@
       <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>96</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="26"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="9" t="s">
         <v>44</v>
       </c>
@@ -4379,7 +4898,7 @@
       <c r="L4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="27" t="s">
         <v>46</v>
       </c>
       <c r="N4" s="9"/>
@@ -4398,7 +4917,7 @@
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="25"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="13" t="s">
         <v>70</v>
       </c>
@@ -4424,7 +4943,7 @@
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="25"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="13" t="s">
         <v>63</v>
       </c>
@@ -4456,7 +4975,7 @@
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="25"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="13" t="s">
         <v>80</v>
       </c>
@@ -4490,7 +5009,7 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="13" t="s">
         <v>80</v>
       </c>
@@ -4526,7 +5045,7 @@
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="25"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="13" t="s">
         <v>89</v>
       </c>
@@ -4560,7 +5079,7 @@
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="25"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="13" t="s">
         <v>58</v>
       </c>
@@ -5163,7 +5682,7 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="17"/>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="28" t="s">
         <v>347</v>
       </c>
       <c r="D39" s="18" t="s">
@@ -5174,14 +5693,14 @@
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
-      <c r="H39" s="31"/>
+      <c r="H39" s="30"/>
       <c r="I39" s="17"/>
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
-      <c r="O39" s="31"/>
+      <c r="O39" s="30"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C40" s="21"/>
@@ -5223,22 +5742,22 @@
   <sheetData>
     <row r="1" spans="2:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="83" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="4"/>
       <c r="O3" s="7"/>
     </row>
@@ -5830,19 +6349,19 @@
       <c r="H20" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="J20" s="61" t="s">
+      <c r="J20" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="61" t="s">
+      <c r="K20" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="61" t="s">
+      <c r="L20" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="62" t="s">
+      <c r="M20" s="59" t="s">
         <v>46</v>
       </c>
       <c r="N20" s="13"/>
@@ -5851,21 +6370,21 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="55"/>
-      <c r="C21" s="56" t="s">
+      <c r="B21" s="52"/>
+      <c r="C21" s="53" t="s">
         <v>234</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="54" t="s">
         <v>279</v>
       </c>
-      <c r="F21" s="57" t="s">
+      <c r="F21" s="54" t="s">
         <v>236</v>
       </c>
-      <c r="G21" s="57"/>
-      <c r="H21" s="66" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="63" t="s">
         <v>46</v>
       </c>
       <c r="I21" s="12" t="s">
@@ -5883,8 +6402,8 @@
       <c r="M21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N21" s="57"/>
-      <c r="O21" s="58"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="55"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
@@ -5901,7 +6420,7 @@
         <v>236</v>
       </c>
       <c r="G22" s="13"/>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="24" t="s">
         <v>46</v>
       </c>
       <c r="I22" s="12" t="s">
@@ -5929,7 +6448,7 @@
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="25">
+      <c r="H23" s="24">
         <v>1</v>
       </c>
       <c r="I23" s="13"/>
@@ -5955,7 +6474,7 @@
         <v>274</v>
       </c>
       <c r="G24" s="13"/>
-      <c r="H24" s="25">
+      <c r="H24" s="24">
         <v>1</v>
       </c>
       <c r="I24" s="21"/>
@@ -5979,7 +6498,7 @@
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="25">
+      <c r="H25" s="24">
         <v>1</v>
       </c>
       <c r="I25" s="13" t="s">
@@ -6005,7 +6524,7 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="24" t="s">
         <v>37</v>
       </c>
       <c r="I26" s="13"/>
@@ -6029,7 +6548,7 @@
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="25" t="s">
+      <c r="H27" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="13" t="s">
@@ -6061,7 +6580,7 @@
         <v>304</v>
       </c>
       <c r="G28" s="13"/>
-      <c r="H28" s="25">
+      <c r="H28" s="24">
         <v>1</v>
       </c>
       <c r="I28" s="13" t="s">
@@ -6097,7 +6616,7 @@
         <v>301</v>
       </c>
       <c r="G29" s="13"/>
-      <c r="H29" s="25">
+      <c r="H29" s="24">
         <v>1</v>
       </c>
       <c r="I29" s="13"/>
@@ -6123,7 +6642,7 @@
         <v>299</v>
       </c>
       <c r="G30" s="13"/>
-      <c r="H30" s="25">
+      <c r="H30" s="24">
         <v>1</v>
       </c>
       <c r="I30" s="13"/>
@@ -6149,7 +6668,7 @@
         <v>299</v>
       </c>
       <c r="G31" s="13"/>
-      <c r="H31" s="25" t="s">
+      <c r="H31" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I31" s="13"/>
@@ -6175,7 +6694,7 @@
         <v>301</v>
       </c>
       <c r="G32" s="13"/>
-      <c r="H32" s="25" t="s">
+      <c r="H32" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I32" s="13"/>
@@ -6201,7 +6720,7 @@
         <v>300</v>
       </c>
       <c r="G33" s="13"/>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I33" s="13"/>
@@ -6225,7 +6744,7 @@
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I34" s="13"/>
@@ -6249,7 +6768,7 @@
       </c>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I35" s="13" t="s">
@@ -6281,7 +6800,7 @@
         <v>303</v>
       </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="25">
+      <c r="H36" s="24">
         <v>1</v>
       </c>
       <c r="I36" s="13" t="s">
@@ -6317,7 +6836,7 @@
         <v>299</v>
       </c>
       <c r="G37" s="13"/>
-      <c r="H37" s="25">
+      <c r="H37" s="24">
         <v>1</v>
       </c>
       <c r="I37" s="13"/>
@@ -6343,7 +6862,7 @@
         <v>301</v>
       </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="25" t="s">
+      <c r="H38" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I38" s="13"/>
@@ -6369,7 +6888,7 @@
         <v>300</v>
       </c>
       <c r="G39" s="13"/>
-      <c r="H39" s="25" t="s">
+      <c r="H39" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I39" s="13"/>
@@ -6393,7 +6912,7 @@
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
-      <c r="H40" s="25" t="s">
+      <c r="H40" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I40" s="13"/>
@@ -6415,7 +6934,7 @@
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="25"/>
+      <c r="H41" s="24"/>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
@@ -6437,7 +6956,7 @@
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="24" t="s">
         <v>37</v>
       </c>
       <c r="I42" s="13"/>
@@ -6459,7 +6978,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I43" s="13" t="s">
@@ -6488,7 +7007,7 @@
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
-      <c r="H44" s="25" t="s">
+      <c r="H44" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I44" s="13" t="s">
@@ -6517,7 +7036,7 @@
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
-      <c r="H45" s="25"/>
+      <c r="H45" s="24"/>
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
@@ -6539,7 +7058,7 @@
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="24" t="s">
         <v>46</v>
       </c>
       <c r="I46" s="13"/>
@@ -6565,7 +7084,7 @@
         <v>299</v>
       </c>
       <c r="G47" s="13"/>
-      <c r="H47" s="25">
+      <c r="H47" s="24">
         <v>1</v>
       </c>
       <c r="I47" s="13"/>
@@ -6591,7 +7110,7 @@
         <v>274</v>
       </c>
       <c r="G48" s="13"/>
-      <c r="H48" s="25">
+      <c r="H48" s="24">
         <v>1</v>
       </c>
       <c r="I48" s="13"/>
@@ -6617,7 +7136,7 @@
         <v>298</v>
       </c>
       <c r="G49" s="13"/>
-      <c r="H49" s="25" t="s">
+      <c r="H49" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I49" s="13"/>
@@ -6641,7 +7160,7 @@
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
-      <c r="H50" s="25">
+      <c r="H50" s="24">
         <v>1</v>
       </c>
       <c r="I50" s="13"/>
@@ -6665,7 +7184,7 @@
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
-      <c r="H51" s="25" t="s">
+      <c r="H51" s="24" t="s">
         <v>46</v>
       </c>
       <c r="I51" s="13"/>
@@ -6691,7 +7210,7 @@
         <v>251</v>
       </c>
       <c r="G52" s="13"/>
-      <c r="H52" s="25">
+      <c r="H52" s="24">
         <v>1</v>
       </c>
       <c r="I52" s="13"/>
@@ -6704,7 +7223,7 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="17"/>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="28" t="s">
         <v>234</v>
       </c>
       <c r="D53" s="18" t="s">
@@ -6717,7 +7236,7 @@
         <v>252</v>
       </c>
       <c r="G53" s="18"/>
-      <c r="H53" s="30">
+      <c r="H53" s="29">
         <v>1</v>
       </c>
       <c r="I53" s="18"/>
@@ -6726,7 +7245,7 @@
       <c r="L53" s="18"/>
       <c r="M53" s="18"/>
       <c r="N53" s="18"/>
-      <c r="O53" s="31"/>
+      <c r="O53" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6763,22 +7282,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="83" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -6846,7 +7365,7 @@
         <v>36</v>
       </c>
       <c r="L4" s="9"/>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="42" t="s">
         <v>37</v>
       </c>
       <c r="N4" s="9"/>
@@ -7027,13 +7546,13 @@
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>218</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="17" t="s">
         <v>81</v>
       </c>
@@ -7091,22 +7610,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="84" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -7129,7 +7648,7 @@
       <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="41" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -7234,39 +7753,39 @@
       <c r="N7" s="13"/>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="2:15" s="52" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
-      <c r="C8" s="46" t="s">
+    <row r="8" spans="2:15" s="50" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="43"/>
+      <c r="C8" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48" t="s">
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="J8" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="K8" s="46" t="s">
+      <c r="K8" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="46" t="s">
+      <c r="L8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="49" t="s">
+      <c r="M8" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="50" t="s">
+      <c r="N8" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="O8" s="51" t="s">
+      <c r="O8" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -7676,7 +8195,7 @@
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="38" t="s">
+      <c r="I26" s="36" t="s">
         <v>43</v>
       </c>
       <c r="J26" s="13"/>
@@ -7700,7 +8219,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="38" t="s">
+      <c r="I27" s="36" t="s">
         <v>43</v>
       </c>
       <c r="J27" s="13"/>
@@ -7722,7 +8241,7 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="38"/>
+      <c r="I28" s="36"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
@@ -7740,7 +8259,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="38"/>
+      <c r="I29" s="36"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
@@ -7758,7 +8277,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="38"/>
+      <c r="I30" s="36"/>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
@@ -7776,7 +8295,7 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="38"/>
+      <c r="I31" s="36"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
@@ -7794,7 +8313,7 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="38"/>
+      <c r="I32" s="36"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
@@ -7812,7 +8331,7 @@
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="38"/>
+      <c r="I33" s="36"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -7832,7 +8351,7 @@
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="15"/>
-      <c r="I34" s="38" t="s">
+      <c r="I34" s="36" t="s">
         <v>43</v>
       </c>
       <c r="J34" s="13"/>
@@ -7852,7 +8371,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="38"/>
+      <c r="I35" s="36"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -7863,20 +8382,20 @@
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
       <c r="C36" s="18"/>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="28" t="s">
         <v>372</v>
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
-      <c r="H36" s="31"/>
+      <c r="H36" s="30"/>
       <c r="I36" s="17"/>
       <c r="J36" s="18"/>
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
-      <c r="O36" s="31"/>
+      <c r="O36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
updating: mapping, ontology and CM
</commit_message>
<xml_diff>
--- a/02-Conceptual_Data_Model/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
+++ b/02-Conceptual_Data_Model/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPaM-Ontology\02-Conceptual_Data_Model\MS-RPaM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPaM-Ontology_v1.1\02-Conceptual_Data_Model\MS-RPaM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1880,7 +1880,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2006,30 +2006,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2088,26 +2064,47 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="2" builtinId="10"/>
-    <cellStyle name="Texto de advertencia" xfId="1" builtinId="11"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2123,7 +2120,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2391,7 +2388,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -2416,7 +2413,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -2431,23 +2428,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
       <c r="H2" s="39"/>
       <c r="I2" s="40"/>
-      <c r="J2" s="71" t="s">
+      <c r="J2" s="117" t="s">
         <v>166</v>
       </c>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
@@ -3304,1603 +3301,1603 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="89" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="89" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" style="89" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" style="89" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="90" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.28515625" style="89" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="89" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="90" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="89"/>
-    <col min="15" max="15" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="89" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="89"/>
+    <col min="1" max="1" width="3.28515625" style="81" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" style="81" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="81" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="81" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="81" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="82" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.28515625" style="81" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="81" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="81" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" style="81" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="82" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="81"/>
+    <col min="15" max="15" width="21.7109375" style="81" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="81" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="81"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="89" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="119" t="s">
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="112"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="82" t="s">
+      <c r="G4" s="74" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="79" t="s">
+      <c r="J4" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="79" t="s">
+      <c r="K4" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="79" t="s">
+      <c r="L4" s="71" t="s">
         <v>9</v>
       </c>
       <c r="M4" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="76" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="91"/>
-      <c r="C5" s="97" t="s">
+      <c r="B5" s="83"/>
+      <c r="C5" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="84" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="92"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="94">
+      <c r="F5" s="84"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="86">
         <v>1</v>
       </c>
-      <c r="I5" s="96" t="s">
+      <c r="I5" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="K5" s="86" t="s">
+      <c r="K5" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="98" t="s">
+      <c r="L5" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="100" t="s">
+      <c r="M5" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="98"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="89" t="s">
+      <c r="N5" s="90"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="81" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="96"/>
-      <c r="C6" s="97" t="s">
+      <c r="B6" s="88"/>
+      <c r="C6" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="89" t="s">
         <v>148</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="F6" s="97"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="F6" s="89"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="85" t="s">
+      <c r="I6" s="77" t="s">
         <v>388</v>
       </c>
-      <c r="J6" s="97" t="s">
+      <c r="J6" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="K6" s="86" t="s">
+      <c r="K6" s="78" t="s">
         <v>389</v>
       </c>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="90" t="s">
         <v>397</v>
       </c>
-      <c r="M6" s="100" t="s">
+      <c r="M6" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="114"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="106"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="96"/>
-      <c r="C7" s="97" t="s">
+      <c r="B7" s="88"/>
+      <c r="C7" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="89" t="s">
         <v>160</v>
       </c>
-      <c r="F7" s="97"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="99" t="s">
+      <c r="F7" s="89"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="85" t="s">
+      <c r="I7" s="77" t="s">
         <v>390</v>
       </c>
-      <c r="J7" s="97" t="s">
+      <c r="J7" s="89" t="s">
         <v>391</v>
       </c>
-      <c r="K7" s="86"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="102" t="s">
+      <c r="K7" s="78"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="N7" s="98"/>
-      <c r="O7" s="114"/>
-      <c r="P7" s="124" t="s">
+      <c r="N7" s="90"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="114" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="96"/>
-      <c r="C8" s="97" t="s">
+      <c r="B8" s="88"/>
+      <c r="C8" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="E8" s="98" t="s">
+      <c r="E8" s="90" t="s">
         <v>158</v>
       </c>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="99">
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="91">
         <v>1</v>
       </c>
-      <c r="I8" s="88" t="s">
+      <c r="I8" s="80" t="s">
         <v>395</v>
       </c>
-      <c r="J8" s="98"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="114"/>
-      <c r="P8" s="124" t="s">
+      <c r="J8" s="90"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="106"/>
+      <c r="P8" s="114" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="96"/>
-      <c r="C9" s="97" t="s">
+      <c r="B9" s="88"/>
+      <c r="C9" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="89" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="89" t="s">
         <v>159</v>
       </c>
-      <c r="F9" s="98" t="s">
+      <c r="F9" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="98"/>
-      <c r="H9" s="99">
+      <c r="G9" s="90"/>
+      <c r="H9" s="91">
         <v>1</v>
       </c>
-      <c r="I9" s="88" t="s">
+      <c r="I9" s="80" t="s">
         <v>395</v>
       </c>
-      <c r="J9" s="98"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="114"/>
-      <c r="P9" s="124" t="s">
+      <c r="J9" s="90"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="106"/>
+      <c r="P9" s="114" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="96"/>
-      <c r="C10" s="97" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="89" t="s">
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="81" t="s">
         <v>392</v>
       </c>
-      <c r="J10" s="97" t="s">
+      <c r="J10" s="89" t="s">
         <v>393</v>
       </c>
-      <c r="K10" s="86" t="s">
+      <c r="K10" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="93" t="s">
+      <c r="L10" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="95" t="s">
+      <c r="M10" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="98"/>
-      <c r="O10" s="114"/>
-      <c r="P10" s="87"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="106"/>
+      <c r="P10" s="79"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="96"/>
-      <c r="C11" s="97" t="s">
+      <c r="B11" s="88"/>
+      <c r="C11" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="88" t="s">
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="80" t="s">
         <v>395</v>
       </c>
-      <c r="J11" s="98"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="98"/>
-      <c r="O11" s="114"/>
-      <c r="P11" s="124" t="s">
+      <c r="J11" s="90"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="106"/>
+      <c r="P11" s="114" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="96"/>
-      <c r="C12" s="97" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="D12" s="89" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="88" t="s">
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="80" t="s">
         <v>395</v>
       </c>
-      <c r="J12" s="98"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="114"/>
-      <c r="P12" s="124" t="s">
+      <c r="J12" s="90"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="106"/>
+      <c r="P12" s="114" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="96"/>
-      <c r="C13" s="97" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
         <v>406</v>
       </c>
-      <c r="D13" s="97" t="s">
+      <c r="D13" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="88" t="s">
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="80" t="s">
         <v>395</v>
       </c>
-      <c r="J13" s="98"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="114"/>
-      <c r="P13" s="124" t="s">
+      <c r="J13" s="90"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="90"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="114" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="96"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="97" t="s">
+      <c r="E14" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="97" t="s">
+      <c r="F14" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="98"/>
-      <c r="H14" s="99">
+      <c r="G14" s="90"/>
+      <c r="H14" s="91">
         <v>1</v>
       </c>
-      <c r="I14" s="96" t="s">
+      <c r="I14" s="88" t="s">
         <v>408</v>
       </c>
-      <c r="J14" s="98" t="s">
+      <c r="J14" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="86" t="s">
+      <c r="K14" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="98" t="s">
+      <c r="L14" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="103" t="s">
+      <c r="M14" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="N14" s="98"/>
-      <c r="O14" s="114"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="106"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="96"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="97" t="s">
+      <c r="E15" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="97" t="s">
+      <c r="F15" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="98"/>
-      <c r="H15" s="99" t="s">
+      <c r="G15" s="90"/>
+      <c r="H15" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="77" t="s">
         <v>405</v>
       </c>
-      <c r="J15" s="98"/>
-      <c r="K15" s="86" t="s">
+      <c r="J15" s="90"/>
+      <c r="K15" s="78" t="s">
         <v>398</v>
       </c>
-      <c r="L15" s="86" t="s">
+      <c r="L15" s="78" t="s">
         <v>396</v>
       </c>
-      <c r="M15" s="102">
+      <c r="M15" s="94">
         <v>1</v>
       </c>
-      <c r="N15" s="98" t="s">
+      <c r="N15" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="O15" s="115" t="s">
+      <c r="O15" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="P15" s="124" t="s">
+      <c r="P15" s="114" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="96"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="97" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="97" t="s">
+      <c r="E16" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="F16" s="97" t="s">
+      <c r="F16" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="G16" s="98"/>
-      <c r="H16" s="99" t="s">
+      <c r="G16" s="90"/>
+      <c r="H16" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="88" t="s">
         <v>409</v>
       </c>
-      <c r="J16" s="98"/>
-      <c r="K16" s="86" t="s">
+      <c r="J16" s="90"/>
+      <c r="K16" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="98" t="s">
+      <c r="L16" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="102">
+      <c r="M16" s="94">
         <v>1</v>
       </c>
-      <c r="N16" s="98" t="s">
+      <c r="N16" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="O16" s="115" t="s">
+      <c r="O16" s="107" t="s">
         <v>394</v>
       </c>
-      <c r="P16" s="113" t="s">
+      <c r="P16" s="105" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="96"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="98" t="s">
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="98" t="s">
+      <c r="E17" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="99">
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="91">
         <v>1</v>
       </c>
-      <c r="I17" s="96" t="s">
+      <c r="I17" s="88" t="s">
         <v>410</v>
       </c>
-      <c r="J17" s="98"/>
-      <c r="K17" s="86" t="s">
+      <c r="J17" s="90"/>
+      <c r="K17" s="78" t="s">
         <v>399</v>
       </c>
-      <c r="L17" s="98" t="s">
+      <c r="L17" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="M17" s="100" t="s">
+      <c r="M17" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="115" t="s">
+      <c r="O17" s="107" t="s">
         <v>400</v>
       </c>
-      <c r="P17" s="113" t="s">
+      <c r="P17" s="105" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="165" x14ac:dyDescent="0.25">
-      <c r="B18" s="96"/>
-      <c r="C18" s="97"/>
-      <c r="D18" s="98" t="s">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="98" t="s">
+      <c r="E18" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="99">
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="91">
         <v>1</v>
       </c>
-      <c r="I18" s="85" t="s">
+      <c r="I18" s="77" t="s">
         <v>418</v>
       </c>
-      <c r="J18" s="98" t="s">
+      <c r="J18" s="90" t="s">
         <v>401</v>
       </c>
-      <c r="K18" s="86" t="s">
+      <c r="K18" s="78" t="s">
         <v>419</v>
       </c>
-      <c r="L18" s="98" t="s">
+      <c r="L18" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="100" t="s">
+      <c r="M18" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N18" s="98"/>
-      <c r="O18" s="115" t="s">
+      <c r="N18" s="90"/>
+      <c r="O18" s="107" t="s">
         <v>420</v>
       </c>
-      <c r="P18" s="125" t="s">
+      <c r="P18" s="114" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="96"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="98" t="s">
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="98" t="s">
+      <c r="E19" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="99">
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="91">
         <v>1</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="88" t="s">
         <v>410</v>
       </c>
-      <c r="J19" s="98" t="s">
+      <c r="J19" s="90" t="s">
         <v>402</v>
       </c>
-      <c r="K19" s="98" t="s">
+      <c r="K19" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="98"/>
-      <c r="M19" s="100" t="s">
+      <c r="L19" s="90"/>
+      <c r="M19" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="N19" s="98"/>
-      <c r="O19" s="114"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="106"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="96"/>
-      <c r="C20" s="97"/>
-      <c r="D20" s="97" t="s">
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="E20" s="97" t="s">
+      <c r="E20" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="F20" s="97"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="99">
+      <c r="F20" s="89"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="91">
         <v>1</v>
       </c>
-      <c r="I20" s="85" t="s">
+      <c r="I20" s="77" t="s">
         <v>443</v>
       </c>
-      <c r="J20" s="97" t="s">
+      <c r="J20" s="89" t="s">
         <v>403</v>
       </c>
-      <c r="K20" s="86" t="s">
+      <c r="K20" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="98"/>
-      <c r="M20" s="102" t="s">
+      <c r="L20" s="90"/>
+      <c r="M20" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="N20" s="98"/>
-      <c r="O20" s="116"/>
-      <c r="P20" s="124" t="s">
+      <c r="N20" s="90"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="114" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="96"/>
-      <c r="C21" s="97"/>
-      <c r="D21" s="98" t="s">
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="90" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="98" t="s">
+      <c r="E21" s="90" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="99" t="s">
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="85" t="s">
+      <c r="I21" s="77" t="s">
         <v>411</v>
       </c>
-      <c r="J21" s="97" t="s">
+      <c r="J21" s="89" t="s">
         <v>404</v>
       </c>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="100" t="s">
+      <c r="K21" s="90"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="N21" s="98"/>
-      <c r="O21" s="114"/>
-      <c r="P21" s="124" t="s">
+      <c r="N21" s="90"/>
+      <c r="O21" s="106"/>
+      <c r="P21" s="114" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="96"/>
-      <c r="C22" s="97"/>
-      <c r="D22" s="98" t="s">
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="98" t="s">
+      <c r="E22" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="F22" s="98" t="s">
+      <c r="F22" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="G22" s="98"/>
-      <c r="H22" s="99" t="s">
+      <c r="G22" s="90"/>
+      <c r="H22" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="96" t="s">
+      <c r="I22" s="88" t="s">
         <v>412</v>
       </c>
-      <c r="J22" s="97" t="s">
+      <c r="J22" s="89" t="s">
         <v>425</v>
       </c>
-      <c r="K22" s="98"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="100">
+      <c r="K22" s="90"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="92">
         <v>1</v>
       </c>
-      <c r="N22" s="85" t="s">
+      <c r="N22" s="77" t="s">
         <v>421</v>
       </c>
-      <c r="O22" s="115" t="s">
+      <c r="O22" s="107" t="s">
         <v>422</v>
       </c>
-      <c r="P22" s="112" t="s">
+      <c r="P22" s="104" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="96"/>
-      <c r="C23" s="97"/>
-      <c r="D23" s="98" t="s">
+      <c r="B23" s="88"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="98" t="s">
+      <c r="E23" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="F23" s="98" t="s">
+      <c r="F23" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="98"/>
-      <c r="H23" s="99" t="s">
+      <c r="G23" s="90"/>
+      <c r="H23" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="96" t="s">
+      <c r="I23" s="88" t="s">
         <v>408</v>
       </c>
-      <c r="J23" s="97" t="s">
+      <c r="J23" s="89" t="s">
         <v>426</v>
       </c>
-      <c r="K23" s="98"/>
-      <c r="L23" s="80"/>
-      <c r="M23" s="100">
+      <c r="K23" s="90"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="92">
         <v>1</v>
       </c>
-      <c r="N23" s="85" t="s">
+      <c r="N23" s="77" t="s">
         <v>424</v>
       </c>
-      <c r="O23" s="115" t="s">
+      <c r="O23" s="107" t="s">
         <v>423</v>
       </c>
-      <c r="P23" s="112" t="s">
+      <c r="P23" s="104" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="96"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="98" t="s">
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="90" t="s">
         <v>115</v>
       </c>
-      <c r="E24" s="98" t="s">
+      <c r="E24" s="90" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="98" t="s">
+      <c r="F24" s="90" t="s">
         <v>120</v>
       </c>
-      <c r="G24" s="98" t="s">
+      <c r="G24" s="90" t="s">
         <v>121</v>
       </c>
-      <c r="H24" s="99" t="s">
+      <c r="H24" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="96" t="s">
+      <c r="I24" s="88" t="s">
         <v>413</v>
       </c>
-      <c r="J24" s="97" t="s">
+      <c r="J24" s="89" t="s">
         <v>427</v>
       </c>
-      <c r="K24" s="98" t="s">
+      <c r="K24" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="L24" s="98" t="s">
+      <c r="L24" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="100">
+      <c r="M24" s="92">
         <v>1</v>
       </c>
-      <c r="N24" s="85" t="s">
+      <c r="N24" s="77" t="s">
         <v>430</v>
       </c>
-      <c r="O24" s="114" t="s">
+      <c r="O24" s="106" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="96"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="98" t="s">
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="90" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="98" t="s">
+      <c r="E25" s="90" t="s">
         <v>117</v>
       </c>
-      <c r="F25" s="98" t="s">
+      <c r="F25" s="90" t="s">
         <v>122</v>
       </c>
-      <c r="G25" s="98" t="s">
+      <c r="G25" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="H25" s="99" t="s">
+      <c r="H25" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="96" t="s">
+      <c r="I25" s="88" t="s">
         <v>416</v>
       </c>
-      <c r="J25" s="97" t="s">
+      <c r="J25" s="89" t="s">
         <v>428</v>
       </c>
-      <c r="K25" s="98" t="s">
+      <c r="K25" s="90" t="s">
         <v>417</v>
       </c>
-      <c r="L25" s="97" t="s">
+      <c r="L25" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="M25" s="100">
+      <c r="M25" s="92">
         <v>1</v>
       </c>
-      <c r="N25" s="85" t="s">
+      <c r="N25" s="77" t="s">
         <v>430</v>
       </c>
-      <c r="O25" s="115" t="s">
+      <c r="O25" s="107" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="96"/>
-      <c r="C26" s="97"/>
-      <c r="D26" s="98" t="s">
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="98" t="s">
+      <c r="E26" s="90" t="s">
         <v>107</v>
       </c>
-      <c r="F26" s="98"/>
-      <c r="G26" s="98"/>
-      <c r="H26" s="99" t="s">
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I26" s="96" t="s">
+      <c r="I26" s="88" t="s">
         <v>432</v>
       </c>
-      <c r="J26" s="97" t="s">
+      <c r="J26" s="89" t="s">
         <v>433</v>
       </c>
-      <c r="K26" s="97" t="s">
+      <c r="K26" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L26" s="97" t="s">
+      <c r="L26" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="M26" s="100" t="s">
+      <c r="M26" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N26" s="98"/>
-      <c r="O26" s="114" t="s">
+      <c r="N26" s="90"/>
+      <c r="O26" s="106" t="s">
         <v>434</v>
       </c>
-      <c r="P26" s="112" t="s">
+      <c r="P26" s="104" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="96"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="98" t="s">
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="E27" s="98" t="s">
+      <c r="E27" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="99" t="s">
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="96" t="s">
+      <c r="I27" s="88" t="s">
         <v>431</v>
       </c>
-      <c r="J27" s="85" t="s">
+      <c r="J27" s="77" t="s">
         <v>435</v>
       </c>
-      <c r="K27" s="97" t="s">
+      <c r="K27" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L27" s="97" t="s">
+      <c r="L27" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="M27" s="100" t="s">
+      <c r="M27" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="N27" s="98"/>
-      <c r="O27" s="114" t="s">
+      <c r="N27" s="90"/>
+      <c r="O27" s="106" t="s">
         <v>437</v>
       </c>
-      <c r="P27" s="112" t="s">
+      <c r="P27" s="104" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="96"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="98" t="s">
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="E28" s="98" t="s">
+      <c r="E28" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="99" t="s">
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="96" t="s">
+      <c r="I28" s="88" t="s">
         <v>440</v>
       </c>
-      <c r="J28" s="85" t="s">
+      <c r="J28" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="K28" s="97" t="s">
+      <c r="K28" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L28" s="98"/>
-      <c r="M28" s="100" t="s">
+      <c r="L28" s="90"/>
+      <c r="M28" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N28" s="98"/>
-      <c r="O28" s="114" t="s">
+      <c r="N28" s="90"/>
+      <c r="O28" s="106" t="s">
         <v>439</v>
       </c>
-      <c r="P28" s="97" t="s">
+      <c r="P28" s="89" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="96"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="98" t="s">
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="98" t="s">
+      <c r="E29" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="F29" s="98" t="s">
+      <c r="F29" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="98"/>
-      <c r="H29" s="99" t="s">
+      <c r="G29" s="90"/>
+      <c r="H29" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I29" s="96" t="s">
+      <c r="I29" s="88" t="s">
         <v>414</v>
       </c>
-      <c r="J29" s="98"/>
-      <c r="K29" s="98" t="s">
+      <c r="J29" s="90"/>
+      <c r="K29" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="L29" s="98" t="s">
+      <c r="L29" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="M29" s="102" t="s">
+      <c r="M29" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="98"/>
-      <c r="O29" s="114"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="106"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="96"/>
-      <c r="C30" s="97"/>
-      <c r="D30" s="98" t="s">
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="98" t="s">
+      <c r="E30" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="F30" s="98"/>
-      <c r="G30" s="98"/>
-      <c r="H30" s="99" t="s">
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="96" t="s">
+      <c r="I30" s="88" t="s">
         <v>414</v>
       </c>
-      <c r="J30" s="98"/>
-      <c r="K30" s="98" t="s">
+      <c r="J30" s="90"/>
+      <c r="K30" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="L30" s="98" t="s">
+      <c r="L30" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="M30" s="102" t="s">
+      <c r="M30" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="N30" s="98"/>
-      <c r="O30" s="114"/>
-      <c r="P30" s="112" t="s">
+      <c r="N30" s="90"/>
+      <c r="O30" s="106"/>
+      <c r="P30" s="104" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="96"/>
-      <c r="C31" s="97"/>
-      <c r="D31" s="98" t="s">
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="98" t="s">
+      <c r="E31" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="99" t="s">
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="96" t="s">
+      <c r="I31" s="88" t="s">
         <v>443</v>
       </c>
-      <c r="J31" s="97" t="s">
+      <c r="J31" s="89" t="s">
         <v>403</v>
       </c>
-      <c r="K31" s="86" t="s">
+      <c r="K31" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="L31" s="98"/>
-      <c r="M31" s="102" t="s">
+      <c r="L31" s="90"/>
+      <c r="M31" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="N31" s="98"/>
-      <c r="O31" s="116"/>
-      <c r="P31" s="124" t="s">
+      <c r="N31" s="90"/>
+      <c r="O31" s="108"/>
+      <c r="P31" s="114" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="96"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="98" t="s">
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="E32" s="98" t="s">
+      <c r="E32" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="99" t="s">
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I32" s="85" t="s">
+      <c r="I32" s="77" t="s">
         <v>442</v>
       </c>
-      <c r="J32" s="97" t="s">
+      <c r="J32" s="89" t="s">
         <v>403</v>
       </c>
-      <c r="K32" s="86" t="s">
+      <c r="K32" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="L32" s="98"/>
-      <c r="M32" s="102" t="s">
+      <c r="L32" s="90"/>
+      <c r="M32" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="N32" s="85" t="s">
+      <c r="N32" s="77" t="s">
         <v>441</v>
       </c>
-      <c r="O32" s="116" t="s">
+      <c r="O32" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="P32" s="124" t="s">
+      <c r="P32" s="114" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="96"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="98" t="s">
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="E33" s="98" t="s">
+      <c r="E33" s="90" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="98"/>
-      <c r="G33" s="98"/>
-      <c r="H33" s="99" t="s">
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="H33" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="I33" s="96" t="s">
+      <c r="I33" s="88" t="s">
         <v>408</v>
       </c>
-      <c r="J33" s="98" t="s">
+      <c r="J33" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="K33" s="98" t="s">
+      <c r="K33" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L33" s="98" t="s">
+      <c r="L33" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="M33" s="102" t="s">
+      <c r="M33" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="N33" s="98"/>
-      <c r="O33" s="114"/>
+      <c r="N33" s="90"/>
+      <c r="O33" s="106"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="96"/>
-      <c r="C34" s="97"/>
-      <c r="D34" s="98" t="s">
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="90" t="s">
         <v>133</v>
       </c>
-      <c r="E34" s="98" t="s">
+      <c r="E34" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="98"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="99" t="s">
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I34" s="96" t="s">
+      <c r="I34" s="88" t="s">
         <v>440</v>
       </c>
-      <c r="J34" s="85" t="s">
+      <c r="J34" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="K34" s="97" t="s">
+      <c r="K34" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L34" s="98"/>
-      <c r="M34" s="100" t="s">
+      <c r="L34" s="90"/>
+      <c r="M34" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N34" s="98"/>
-      <c r="O34" s="114" t="s">
+      <c r="N34" s="90"/>
+      <c r="O34" s="106" t="s">
         <v>439</v>
       </c>
-      <c r="P34" s="97" t="s">
+      <c r="P34" s="89" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="96"/>
-      <c r="C35" s="97"/>
-      <c r="D35" s="98" t="s">
+      <c r="B35" s="88"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="E35" s="98" t="s">
+      <c r="E35" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="F35" s="98"/>
-      <c r="G35" s="98"/>
-      <c r="H35" s="99" t="s">
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="96" t="s">
+      <c r="I35" s="88" t="s">
         <v>458</v>
       </c>
-      <c r="J35" s="97" t="s">
+      <c r="J35" s="89" t="s">
         <v>459</v>
       </c>
-      <c r="K35" s="97" t="s">
+      <c r="K35" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="L35" s="97" t="s">
+      <c r="L35" s="89" t="s">
         <v>417</v>
       </c>
-      <c r="M35" s="102" t="s">
+      <c r="M35" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="N35" s="98"/>
-      <c r="O35" s="114" t="s">
+      <c r="N35" s="90"/>
+      <c r="O35" s="106" t="s">
         <v>460</v>
       </c>
-      <c r="P35" s="112" t="s">
+      <c r="P35" s="104" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="96"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="98" t="s">
+      <c r="B36" s="88"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="99" t="s">
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
+      <c r="H36" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="96" t="s">
+      <c r="I36" s="88" t="s">
         <v>440</v>
       </c>
-      <c r="J36" s="85" t="s">
+      <c r="J36" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="K36" s="97" t="s">
+      <c r="K36" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L36" s="98"/>
-      <c r="M36" s="100" t="s">
+      <c r="L36" s="90"/>
+      <c r="M36" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N36" s="98"/>
-      <c r="O36" s="114" t="s">
+      <c r="N36" s="90"/>
+      <c r="O36" s="106" t="s">
         <v>463</v>
       </c>
-      <c r="P36" s="112" t="s">
+      <c r="P36" s="104" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="96"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="98" t="s">
+      <c r="B37" s="88"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="98"/>
-      <c r="F37" s="98"/>
-      <c r="G37" s="98"/>
-      <c r="H37" s="99" t="s">
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="96" t="s">
+      <c r="I37" s="88" t="s">
         <v>440</v>
       </c>
-      <c r="J37" s="85" t="s">
+      <c r="J37" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="K37" s="97" t="s">
+      <c r="K37" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L37" s="98"/>
-      <c r="M37" s="100" t="s">
+      <c r="L37" s="90"/>
+      <c r="M37" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N37" s="98"/>
-      <c r="O37" s="114" t="s">
+      <c r="N37" s="90"/>
+      <c r="O37" s="106" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="96"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="98" t="s">
+      <c r="B38" s="88"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="98"/>
-      <c r="F38" s="98"/>
-      <c r="G38" s="98"/>
-      <c r="H38" s="99" t="s">
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="90"/>
+      <c r="H38" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I38" s="96" t="s">
+      <c r="I38" s="88" t="s">
         <v>440</v>
       </c>
-      <c r="J38" s="85" t="s">
+      <c r="J38" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="K38" s="97" t="s">
+      <c r="K38" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L38" s="98"/>
-      <c r="M38" s="100" t="s">
+      <c r="L38" s="90"/>
+      <c r="M38" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N38" s="98"/>
-      <c r="O38" s="114" t="s">
+      <c r="N38" s="90"/>
+      <c r="O38" s="106" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="96"/>
-      <c r="C39" s="97"/>
-      <c r="D39" s="98" t="s">
+      <c r="B39" s="88"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="E39" s="98" t="s">
+      <c r="E39" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="98"/>
-      <c r="G39" s="98"/>
-      <c r="H39" s="99" t="s">
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I39" s="104" t="s">
+      <c r="I39" s="96" t="s">
         <v>415</v>
       </c>
-      <c r="J39" s="97"/>
-      <c r="K39" s="97" t="s">
+      <c r="J39" s="89"/>
+      <c r="K39" s="89" t="s">
         <v>175</v>
       </c>
-      <c r="L39" s="97"/>
-      <c r="M39" s="102" t="s">
+      <c r="L39" s="89"/>
+      <c r="M39" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="N39" s="97"/>
-      <c r="O39" s="117"/>
+      <c r="N39" s="89"/>
+      <c r="O39" s="109"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="96"/>
-      <c r="C40" s="97"/>
-      <c r="D40" s="98" t="s">
+      <c r="B40" s="88"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="E40" s="98" t="s">
+      <c r="E40" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="F40" s="98"/>
-      <c r="G40" s="98"/>
-      <c r="H40" s="99" t="s">
+      <c r="F40" s="90"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="I40" s="96" t="s">
+      <c r="I40" s="88" t="s">
         <v>440</v>
       </c>
-      <c r="J40" s="85" t="s">
+      <c r="J40" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="K40" s="97" t="s">
+      <c r="K40" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="L40" s="98"/>
-      <c r="M40" s="102" t="s">
+      <c r="L40" s="90"/>
+      <c r="M40" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="N40" s="98"/>
-      <c r="O40" s="114"/>
+      <c r="N40" s="90"/>
+      <c r="O40" s="106"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="105"/>
-      <c r="C41" s="106"/>
-      <c r="D41" s="107" t="s">
+      <c r="B41" s="97"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="E41" s="107" t="s">
+      <c r="E41" s="99" t="s">
         <v>108</v>
       </c>
-      <c r="F41" s="107"/>
-      <c r="G41" s="107"/>
-      <c r="H41" s="108">
+      <c r="F41" s="99"/>
+      <c r="G41" s="99"/>
+      <c r="H41" s="100">
         <v>1</v>
       </c>
-      <c r="I41" s="126" t="s">
+      <c r="I41" s="115" t="s">
         <v>395</v>
       </c>
-      <c r="J41" s="107"/>
-      <c r="K41" s="107"/>
-      <c r="L41" s="107"/>
-      <c r="M41" s="109"/>
-      <c r="N41" s="107"/>
-      <c r="O41" s="118" t="s">
+      <c r="J41" s="99"/>
+      <c r="K41" s="99"/>
+      <c r="L41" s="99"/>
+      <c r="M41" s="101"/>
+      <c r="N41" s="99"/>
+      <c r="O41" s="110" t="s">
         <v>464</v>
       </c>
-      <c r="P41" s="112" t="s">
+      <c r="P41" s="104" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="91"/>
-      <c r="C42" s="93" t="s">
+      <c r="B42" s="83"/>
+      <c r="C42" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="D42" s="92" t="s">
+      <c r="D42" s="84" t="s">
         <v>305</v>
       </c>
-      <c r="E42" s="92" t="s">
+      <c r="E42" s="84" t="s">
         <v>313</v>
       </c>
-      <c r="F42" s="93" t="s">
+      <c r="F42" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="G42" s="93"/>
-      <c r="H42" s="94"/>
-      <c r="I42" s="127" t="s">
+      <c r="G42" s="85"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="116" t="s">
         <v>395</v>
       </c>
-      <c r="J42" s="93"/>
-      <c r="K42" s="93"/>
-      <c r="L42" s="93"/>
-      <c r="M42" s="95"/>
-      <c r="N42" s="93"/>
-      <c r="O42" s="111"/>
-      <c r="P42" s="123" t="s">
+      <c r="J42" s="85"/>
+      <c r="K42" s="85"/>
+      <c r="L42" s="85"/>
+      <c r="M42" s="87"/>
+      <c r="N42" s="85"/>
+      <c r="O42" s="103"/>
+      <c r="P42" s="113" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="96"/>
-      <c r="C43" s="98" t="s">
+      <c r="B43" s="88"/>
+      <c r="C43" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="D43" s="97" t="s">
+      <c r="D43" s="89" t="s">
         <v>306</v>
       </c>
-      <c r="E43" s="97" t="s">
+      <c r="E43" s="89" t="s">
         <v>314</v>
       </c>
-      <c r="F43" s="97" t="s">
+      <c r="F43" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="G43" s="98"/>
-      <c r="H43" s="99"/>
-      <c r="I43" s="127" t="s">
+      <c r="G43" s="90"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="116" t="s">
         <v>395</v>
       </c>
-      <c r="J43" s="98"/>
-      <c r="K43" s="98"/>
-      <c r="L43" s="98"/>
-      <c r="M43" s="100"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="101"/>
-      <c r="P43" s="87" t="s">
+      <c r="J43" s="90"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="90"/>
+      <c r="M43" s="92"/>
+      <c r="N43" s="90"/>
+      <c r="O43" s="93"/>
+      <c r="P43" s="79" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="96"/>
-      <c r="C44" s="98" t="s">
+      <c r="B44" s="88"/>
+      <c r="C44" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="D44" s="97" t="s">
+      <c r="D44" s="89" t="s">
         <v>308</v>
       </c>
-      <c r="E44" s="97" t="s">
+      <c r="E44" s="89" t="s">
         <v>319</v>
       </c>
-      <c r="F44" s="97" t="s">
+      <c r="F44" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="98"/>
-      <c r="H44" s="99" t="s">
+      <c r="G44" s="90"/>
+      <c r="H44" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="97" t="s">
+      <c r="I44" s="89" t="s">
         <v>327</v>
       </c>
-      <c r="J44" s="98" t="s">
+      <c r="J44" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="K44" s="98" t="s">
+      <c r="K44" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="L44" s="98"/>
-      <c r="M44" s="102" t="s">
+      <c r="L44" s="90"/>
+      <c r="M44" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="N44" s="98"/>
-      <c r="O44" s="101"/>
+      <c r="N44" s="90"/>
+      <c r="O44" s="93"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="96"/>
-      <c r="C45" s="98" t="s">
+      <c r="B45" s="88"/>
+      <c r="C45" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="D45" s="97" t="s">
+      <c r="D45" s="89" t="s">
         <v>307</v>
       </c>
-      <c r="E45" s="98" t="s">
+      <c r="E45" s="90" t="s">
         <v>318</v>
       </c>
-      <c r="F45" s="97" t="s">
+      <c r="F45" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="G45" s="98"/>
-      <c r="H45" s="99" t="s">
+      <c r="G45" s="90"/>
+      <c r="H45" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="I45" s="96" t="s">
+      <c r="I45" s="88" t="s">
         <v>468</v>
       </c>
-      <c r="J45" s="98"/>
-      <c r="K45" s="98"/>
-      <c r="L45" s="98"/>
-      <c r="M45" s="100" t="s">
+      <c r="J45" s="90"/>
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
+      <c r="M45" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N45" s="98"/>
-      <c r="O45" s="118" t="s">
+      <c r="N45" s="90"/>
+      <c r="O45" s="110" t="s">
         <v>471</v>
       </c>
-      <c r="P45" s="112" t="s">
+      <c r="P45" s="104" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="96"/>
-      <c r="C46" s="98" t="s">
+      <c r="B46" s="88"/>
+      <c r="C46" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="D46" s="97" t="s">
+      <c r="D46" s="89" t="s">
         <v>309</v>
       </c>
-      <c r="E46" s="98" t="s">
+      <c r="E46" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="F46" s="97" t="s">
+      <c r="F46" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="G46" s="98"/>
-      <c r="H46" s="99" t="s">
+      <c r="G46" s="90"/>
+      <c r="H46" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I46" s="96" t="s">
+      <c r="I46" s="88" t="s">
         <v>468</v>
       </c>
-      <c r="J46" s="98"/>
-      <c r="K46" s="98"/>
-      <c r="L46" s="98"/>
-      <c r="M46" s="100" t="s">
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
+      <c r="M46" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="N46" s="98"/>
-      <c r="O46" s="118" t="s">
+      <c r="N46" s="90"/>
+      <c r="O46" s="110" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="96"/>
-      <c r="C47" s="98" t="s">
+      <c r="B47" s="88"/>
+      <c r="C47" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="D47" s="97" t="s">
+      <c r="D47" s="89" t="s">
         <v>310</v>
       </c>
-      <c r="E47" s="98"/>
-      <c r="F47" s="98"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="99"/>
-      <c r="I47" s="85" t="s">
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
+      <c r="H47" s="91"/>
+      <c r="I47" s="77" t="s">
         <v>472</v>
       </c>
-      <c r="J47" s="98" t="s">
+      <c r="J47" s="90" t="s">
         <v>473</v>
       </c>
-      <c r="K47" s="98"/>
-      <c r="L47" s="98"/>
-      <c r="M47" s="100"/>
-      <c r="N47" s="98"/>
-      <c r="O47" s="101"/>
-      <c r="P47" s="112" t="s">
+      <c r="K47" s="90"/>
+      <c r="L47" s="90"/>
+      <c r="M47" s="92"/>
+      <c r="N47" s="90"/>
+      <c r="O47" s="93"/>
+      <c r="P47" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="96"/>
-      <c r="C48" s="98" t="s">
+      <c r="B48" s="88"/>
+      <c r="C48" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="D48" s="97" t="s">
+      <c r="D48" s="89" t="s">
         <v>311</v>
       </c>
-      <c r="E48" s="98" t="s">
+      <c r="E48" s="90" t="s">
         <v>315</v>
       </c>
-      <c r="F48" s="98"/>
-      <c r="G48" s="98"/>
-      <c r="H48" s="99"/>
-      <c r="I48" s="96" t="s">
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
+      <c r="H48" s="91"/>
+      <c r="I48" s="88" t="s">
         <v>475</v>
       </c>
-      <c r="J48" s="98" t="s">
+      <c r="J48" s="90" t="s">
         <v>477</v>
       </c>
-      <c r="K48" s="98"/>
-      <c r="L48" s="98"/>
-      <c r="M48" s="100" t="s">
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
+      <c r="M48" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="N48" s="98"/>
-      <c r="O48" s="118" t="s">
+      <c r="N48" s="90"/>
+      <c r="O48" s="110" t="s">
         <v>481</v>
       </c>
-      <c r="P48" s="112" t="s">
+      <c r="P48" s="104" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="96"/>
-      <c r="C49" s="98"/>
-      <c r="D49" s="97"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="99"/>
-      <c r="I49" s="96" t="s">
+      <c r="B49" s="88"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="90"/>
+      <c r="H49" s="91"/>
+      <c r="I49" s="88" t="s">
         <v>476</v>
       </c>
-      <c r="J49" s="98" t="s">
+      <c r="J49" s="90" t="s">
         <v>478</v>
       </c>
-      <c r="K49" s="98"/>
-      <c r="L49" s="98"/>
-      <c r="M49" s="100" t="s">
+      <c r="K49" s="90"/>
+      <c r="L49" s="90"/>
+      <c r="M49" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="N49" s="98"/>
-      <c r="O49" s="101"/>
+      <c r="N49" s="90"/>
+      <c r="O49" s="93"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="105"/>
-      <c r="C50" s="107" t="s">
+      <c r="B50" s="97"/>
+      <c r="C50" s="99" t="s">
         <v>234</v>
       </c>
-      <c r="D50" s="106" t="s">
+      <c r="D50" s="98" t="s">
         <v>312</v>
       </c>
-      <c r="E50" s="107" t="s">
+      <c r="E50" s="99" t="s">
         <v>316</v>
       </c>
-      <c r="F50" s="107" t="s">
+      <c r="F50" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="G50" s="107"/>
-      <c r="H50" s="108"/>
-      <c r="I50" s="96" t="s">
+      <c r="G50" s="99"/>
+      <c r="H50" s="100"/>
+      <c r="I50" s="88" t="s">
         <v>474</v>
       </c>
-      <c r="J50" s="107" t="s">
+      <c r="J50" s="99" t="s">
         <v>479</v>
       </c>
-      <c r="K50" s="107"/>
-      <c r="L50" s="107"/>
-      <c r="M50" s="109" t="s">
+      <c r="K50" s="99"/>
+      <c r="L50" s="99"/>
+      <c r="M50" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="N50" s="107"/>
-      <c r="O50" s="110"/>
+      <c r="N50" s="99"/>
+      <c r="O50" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4920,11 +4917,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="5.140625" customWidth="1"/>
@@ -4942,22 +4939,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76" t="s">
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -5850,11 +5847,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" customWidth="1"/>
@@ -5873,22 +5870,22 @@
   <sheetData>
     <row r="1" spans="2:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="76" t="s">
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
       <c r="N3" s="4"/>
       <c r="O3" s="7"/>
     </row>
@@ -7396,7 +7393,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
@@ -7413,22 +7410,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76" t="s">
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>
@@ -7722,7 +7719,7 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.140625" customWidth="1"/>
@@ -7741,22 +7738,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="77" t="s">
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
       <c r="N2" s="4"/>
       <c r="O2" s="7"/>
     </row>

</xml_diff>